<commit_message>
improve margin of safety scraping
</commit_message>
<xml_diff>
--- a/Russell 2000 DCFs.xlsx
+++ b/Russell 2000 DCFs.xlsx
@@ -549,8 +549,10 @@
       <c r="N2" t="n">
         <v>1.55</v>
       </c>
-      <c r="O2" t="n">
-        <v>-69</v>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
     </row>
     <row r="3">

</xml_diff>